<commit_message>
Funkčný cron aj aktualizácia as DB
</commit_message>
<xml_diff>
--- a/app/3.xlsx
+++ b/app/3.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="390" yWindow="600" windowWidth="12135" windowHeight="5070"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Erik Ladňák
 Jakub Rončák
@@ -37,29 +36,32 @@
 Webstránka 10515€
 Marináda 32€</t>
   </si>
+  <si>
+    <t>Erik Ladňá
+Jakub Rončák
+Elf René</t>
+  </si>
+  <si>
+    <t>ladnak.erik@gmail.co
+jakub.roncak@gmail.com
+elf@rene.sk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -70,17 +72,20 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -94,39 +99,35 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,107 +417,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="true" style="0"/>
-    <col min="2" max="2" width="23.7109375" customWidth="true" style="0"/>
-    <col min="3" max="3" width="10.140625" customWidth="true" style="0"/>
-    <col min="5" max="5" width="18.28515625" customWidth="true" style="0"/>
-    <col min="8" max="8" width="10.28515625" customWidth="true" style="0"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" customHeight="1" ht="60">
+    <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="3"/>
-      <c r="G1"/>
       <c r="H1" s="3"/>
-      <c r="I1"/>
       <c r="J1" s="3"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-    </row>
-    <row r="2" spans="1:17" customHeight="1" ht="60">
+    </row>
+    <row r="2" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
-      <c r="G2"/>
       <c r="H2" s="3"/>
-      <c r="I2"/>
       <c r="J2" s="3"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-    </row>
-    <row r="3" spans="1:17" customHeight="1" ht="60">
+    </row>
+    <row r="3" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
-      <c r="G3"/>
       <c r="H3" s="3"/>
-      <c r="I3"/>
       <c r="J3" s="3"/>
-      <c r="K3"/>
-      <c r="L3"/>
       <c r="M3" s="3"/>
-      <c r="N3"/>
       <c r="O3" s="3"/>
-      <c r="P3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" customHeight="1" ht="60">
+    <row r="4" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
-      <c r="G4"/>
       <c r="H4" s="3"/>
-      <c r="I4"/>
       <c r="J4" s="3"/>
-      <c r="K4"/>
-      <c r="L4"/>
       <c r="M4" s="3"/>
-      <c r="N4"/>
       <c r="O4" s="3"/>
-      <c r="P4"/>
       <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:17" customHeight="1" ht="60">
+    <row r="5" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6">
         <v>43703</v>
@@ -534,7 +502,7 @@
       <c r="O5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="1:17" customHeight="1" ht="60">
+    <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -554,7 +522,7 @@
       <c r="H6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:17" customHeight="1" ht="60">
+    <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -574,28 +542,28 @@
       <c r="H7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="F8" s="3"/>
       <c r="H8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="F9" s="3"/>
       <c r="H9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="F10" s="3"/>
       <c r="H10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="F11" s="3"/>
@@ -603,82 +571,43 @@
       <c r="J11" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId_hyperlink_1"/>
-    <hyperlink ref="B2" r:id="rId_hyperlink_2"/>
-    <hyperlink ref="B3" r:id="rId_hyperlink_3"/>
-    <hyperlink ref="B4" r:id="rId_hyperlink_4"/>
-    <hyperlink ref="B5" r:id="rId_hyperlink_5"/>
-    <hyperlink ref="B6" r:id="rId_hyperlink_6"/>
-    <hyperlink ref="B7" r:id="rId_hyperlink_7"/>
+    <hyperlink ref="B1" r:id="rId1" display="mailto:ladnak.erik@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="mailto:ladnak.erik@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="mailto:ladnak.erik@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId4" display="mailto:ladnak.erik@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId5" display="ladnak.erik@gmail.com_x000a_jakub.roncak@gmail.com_x000a_elf@rene.sk"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
   </hyperlinks>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>